<commit_message>
4/5v2 I cleaned up the transitions between stages, ready for presentation
</commit_message>
<xml_diff>
--- a/1.xlsx
+++ b/1.xlsx
@@ -6,13 +6,13 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Geo 121" r:id="rId3" sheetId="1"/>
+    <sheet name="BUS 333" r:id="rId3" sheetId="1"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -33,6 +33,21 @@
   </si>
   <si>
     <t>35</t>
+  </si>
+  <si>
+    <t>179</t>
+  </si>
+  <si>
+    <t>128</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>255</t>
+  </si>
+  <si>
+    <t>204</t>
   </si>
 </sst>
 </file>
@@ -94,13 +109,13 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="E1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
curve & graph & add and delete assignment/homework is working. Need to finish search and print
</commit_message>
<xml_diff>
--- a/1.xlsx
+++ b/1.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="41">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -275,7 +275,7 @@
         <v>6</v>
       </c>
       <c r="F6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7">
@@ -295,7 +295,7 @@
         <v>27</v>
       </c>
       <c r="F7" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8">
@@ -303,7 +303,7 @@
         <v>6</v>
       </c>
       <c r="F8" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9">
@@ -323,7 +323,7 @@
         <v>39</v>
       </c>
       <c r="F9" t="s">
-        <v>37</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>